<commit_message>
clean up and submit
</commit_message>
<xml_diff>
--- a/Data/Tables.xlsx
+++ b/Data/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxiang\Desktop\REU-Android-Spring2022\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7FBA6C-EE0E-475D-8711-C39A5F6F259B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1509821E-4CEF-46CB-9532-63E5618BFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BenignStats" sheetId="1" r:id="rId1"/>
@@ -103,16 +103,20 @@
     <t>Nan</t>
   </si>
   <si>
-    <t>installation-time incompatible ratio (Benign 2010-2019)</t>
-  </si>
-  <si>
-    <t>run-time incompatible ratio (Benign 2010-2019)</t>
-  </si>
-  <si>
-    <t>installation-time incompatible ratio (Malware 2018-2019)</t>
-  </si>
-  <si>
-    <t>run-time incompatible ratio (Malware 2010-2019)</t>
+    <t>installation-time incompatible ratio 
+(Benign 2010-2019)</t>
+  </si>
+  <si>
+    <t>run-time incompatible ratio 
+(Benign 2010-2019)</t>
+  </si>
+  <si>
+    <t>installation-time incompatible ratio 
+(Malware 2018-2019)</t>
+  </si>
+  <si>
+    <t>run-time incompatible ratio 
+(Malware 2010-2019)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -192,18 +196,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -487,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -497,27 +506,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2">
         <v>2010</v>
       </c>
@@ -548,7 +557,7 @@
       <c r="L3" s="2">
         <v>2019</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -653,27 +662,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="2">
         <v>2010</v>
       </c>
@@ -704,7 +713,7 @@
       <c r="L3" s="2">
         <v>2019</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="6"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -782,13 +791,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B713172E-0CE1-46FA-AD68-DF38BC7C9600}">
   <dimension ref="B2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
@@ -813,187 +822,187 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>6.8580000000000004E-3</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="5">
         <v>0.399003</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>-0.46011600000000002</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>-0.19988400000000001</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>-5.9249999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>-4.548E-3</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>0.30102299999999999</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>-0.33309499999999997</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>-0.110004</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <v>-2.2058000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="5">
         <v>-0.28972300000000001</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>0.10674400000000001</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>-0.258521</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <v>-0.49645400000000001</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <v>-4.5740000000000003E-2</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <v>0.16828499999999999</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="4">
         <v>0.181223</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="4">
         <v>-0.21257499999999999</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>-5.7606999999999998E-2</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <v>-0.21249100000000001</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1014,163 +1023,163 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <v>-0.40721600000000002</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>-0.16056200000000001</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>4.8492E-2</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <v>-0.43172899999999997</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <v>2.6228999999999999E-2</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <v>-0.297657</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>-7.8220999999999999E-2</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>2.7079999999999999E-3</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="4">
         <v>-0.31161699999999998</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="4">
         <v>3.3715000000000002E-2</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <v>-6.1679999999999999E-2</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <v>9.0259999999999993E-3</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>-3.3328000000000003E-2</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>-7.0989999999999998E-2</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <v>-4.6474000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="5">
         <v>-0.21617800000000001</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="4">
         <v>0.17680100000000001</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="4">
         <v>-0.271787</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <v>-0.32069399999999998</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="4">
         <v>8.2922999999999997E-2</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="4">
         <v>-0.181285</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="4">
         <v>8.7320999999999996E-2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="4">
         <v>-0.13291600000000001</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="4">
         <v>-0.15376200000000001</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="4">
         <v>0.114699</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <v>-0.17250299999999999</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="4">
         <v>0.14956800000000001</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="4">
         <v>-0.22701499999999999</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <v>-0.26285700000000001</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="4">
         <v>6.2886999999999998E-2</v>
       </c>
     </row>

</xml_diff>